<commit_message>
back up go files (cause of GoCV dependencies)
</commit_message>
<xml_diff>
--- a/step_by_step_mlp.xlsx
+++ b/step_by_step_mlp.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Step_1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Step_2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Step_3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,14 +22,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="42">
   <si>
     <t xml:space="preserve">Input</t>
   </si>
   <si>
+    <t xml:space="preserve">Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derivative of activation func</t>
+  </si>
+  <si>
     <t xml:space="preserve">in0</t>
   </si>
   <si>
+    <t xml:space="preserve">Tanh(x)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 — Tanh(x) * Tanh(x)</t>
+  </si>
+  <si>
     <t xml:space="preserve">in1</t>
   </si>
   <si>
@@ -53,6 +66,9 @@
     <t xml:space="preserve">Activated</t>
   </si>
   <si>
+    <t xml:space="preserve">Derevative</t>
+  </si>
+  <si>
     <t xml:space="preserve">out0</t>
   </si>
   <si>
@@ -92,13 +108,13 @@
     <t xml:space="preserve">Learning rate</t>
   </si>
   <si>
-    <t xml:space="preserve">Layer 3 (deltas)</t>
+    <t xml:space="preserve">Layer 3 (errors)</t>
   </si>
   <si>
     <t xml:space="preserve">delta0</t>
   </si>
   <si>
-    <t xml:space="preserve">Layer 2 (deltas)</t>
+    <t xml:space="preserve">Layer 2 (errors)</t>
   </si>
   <si>
     <t xml:space="preserve">delta1</t>
@@ -107,7 +123,7 @@
     <t xml:space="preserve">delta2</t>
   </si>
   <si>
-    <t xml:space="preserve">Layer 1 (deltas)</t>
+    <t xml:space="preserve">Layer 1 (errors)</t>
   </si>
   <si>
     <t xml:space="preserve">Layer 1 (delta weights)</t>
@@ -141,12 +157,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -163,13 +178,132 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -202,7 +336,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -210,8 +344,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -235,59 +384,131 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -299,7 +520,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF7B59"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -315,7 +536,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FFACB20C"/>
@@ -344,8 +565,8 @@
   </sheetPr>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -353,7 +574,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.1"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -361,34 +582,48 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.2</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
+      <c r="A5" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>-1</v>
@@ -399,10 +634,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -412,50 +647,61 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">C6*B2+D6*B3</f>
         <v>0.3</v>
       </c>
       <c r="C10" s="0" t="n">
-        <f aca="false">1/(1+EXP(-B10))</f>
-        <v>0.574442516811659</v>
+        <f aca="false">TANH(B10)</f>
+        <v>0.291312612451591</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">1-C10*C10</f>
+        <v>0.915136961826629</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">C7*B2+D7*B3</f>
         <v>1.2</v>
       </c>
       <c r="C11" s="0" t="n">
-        <f aca="false">1/(1+EXP(-B11))</f>
-        <v>0.768524783499018</v>
+        <f aca="false">TANH(B11)</f>
+        <v>0.833654607012155</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">1-C11*C11</f>
+        <v>0.305019996207409</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>12</v>
+      <c r="A13" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>-1</v>
@@ -466,10 +712,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
@@ -480,10 +726,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>3</v>
@@ -493,70 +739,85 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="4" t="s">
-        <v>9</v>
+      <c r="A18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">C14*C10+D14*C11</f>
-        <v>0.962607050186376</v>
+        <v>1.37599660157272</v>
       </c>
       <c r="C19" s="0" t="n">
-        <f aca="false">1/(1+EXP(-B19))</f>
-        <v>0.723643476259143</v>
+        <f aca="false">TANH(B19)</f>
+        <v>0.880051639598856</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">1-C19*C19</f>
+        <v>0.225509111639364</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B20" s="0" t="n">
         <f aca="false">C15*C10+D15*C11</f>
-        <v>1.34296730031068</v>
+        <v>1.12496721946375</v>
       </c>
       <c r="C20" s="0" t="n">
-        <f aca="false">1/(1+EXP(-B20))</f>
-        <v>0.792977489387612</v>
+        <f aca="false">TANH(B20)</f>
+        <v>0.809289759575022</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">1-C20*C20</f>
+        <v>0.345050085047003</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B21" s="0" t="n">
         <f aca="false">C16*C10+D16*C11</f>
-        <v>0.186277983436942</v>
+        <v>-0.793371376669538</v>
       </c>
       <c r="C21" s="0" t="n">
-        <f aca="false">1/(1+EXP(-B21))</f>
-        <v>0.546435300024219</v>
+        <f aca="false">TANH(B21)</f>
+        <v>-0.660314675296505</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">1-C21*C21</f>
+        <v>0.563984529588071</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>17</v>
+      <c r="A23" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>1</v>
@@ -569,299 +830,322 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>9</v>
+      <c r="A26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B27" s="0" t="n">
         <f aca="false">D24*C19+E24*C20+F24*C21</f>
-        <v>4.49533965513124</v>
+        <v>-0.14262754243712</v>
       </c>
       <c r="C27" s="0" t="n">
-        <f aca="false">1/(1+EXP(-B27))</f>
-        <v>0.988962301412063</v>
+        <f aca="false">TANH(B27)</f>
+        <v>-0.141668208722161</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">1-C27*C27</f>
+        <v>0.979930118637454</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B31" s="0" t="n">
-        <f aca="false">B29-C27</f>
-        <v>-0.588962301412063</v>
+        <f aca="false">C27-B29</f>
+        <v>-0.541668208722161</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="2" t="n">
-        <v>0.85</v>
+        <v>27</v>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>0.01</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
-        <v>23</v>
+      <c r="A35" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <f aca="false">B36*D19</f>
+        <v>-0.119699558134715</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <f aca="false">B36*D20</f>
+        <v>-0.183151547244455</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <f aca="false">B36*D21</f>
+        <v>-0.29936129185976</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B36" s="0" t="n">
-        <f aca="false">B31*C27*(1-C27)</f>
-        <v>-0.00642903462011323</v>
+        <f aca="false">B31*D27</f>
+        <v>-0.530796992035244</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>25</v>
+      <c r="A38" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D39" s="0" t="n">
-        <f aca="false">B36*D24*C19*(1-C19)</f>
-        <v>-0.00128570145909604</v>
+        <f aca="false">B36*D24*D19</f>
+        <v>-0.119699558134715</v>
       </c>
       <c r="E39" s="0" t="n">
-        <f aca="false">B36*E24*C20*(1-C20)</f>
-        <v>-0.00211083453094233</v>
+        <f aca="false">B36*E24*D20</f>
+        <v>-0.366303094488909</v>
       </c>
       <c r="F39" s="0" t="n">
-        <f aca="false">B36*F24*C21*(1-C21)</f>
-        <v>-0.00637358452855281</v>
+        <f aca="false">B36*F24*D21</f>
+        <v>-1.19744516743904</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>28</v>
+      <c r="A41" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C42" s="0" t="n">
-        <f aca="false">(D39*C14+E39*C15+F39*C16)*C10*(1-C10)</f>
-        <v>-0.00487593777746858</v>
+        <f aca="false">(D39*C14+E39*C15+F39*C16)*D10</f>
+        <v>-3.51315500848731</v>
       </c>
       <c r="D42" s="0" t="n">
-        <f aca="false">(D39*D14+E39*D15+F39*D16)*C11*(1-C11)</f>
-        <v>0.00143470649725478</v>
+        <f aca="false">(D39*D14+E39*D15+F39*D16)*D11</f>
+        <v>0.545738154833346</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>30</v>
+      <c r="A44" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C45" s="0" t="n">
-        <f aca="false">B33*B2*C42</f>
-        <v>-0.000828909422169658</v>
+        <f aca="false">-B33*B2*C42</f>
+        <v>0.00702631001697462</v>
       </c>
       <c r="D45" s="0" t="n">
-        <f aca="false">B33*B3*C42</f>
-        <v>-0.00207227355542415</v>
+        <f aca="false">-B33*B3*C42</f>
+        <v>0.0175657750424366</v>
       </c>
       <c r="F45" s="0" t="n">
         <f aca="false">C6+C45</f>
-        <v>-1.00082890942217</v>
+        <v>-0.992973689983025</v>
       </c>
       <c r="G45" s="0" t="n">
         <f aca="false">D6+D45</f>
-        <v>0.997927726444576</v>
+        <v>1.01756577504244</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C46" s="0" t="n">
-        <f aca="false">B33*B2*D42</f>
-        <v>0.000243900104533313</v>
+        <f aca="false">-B33*B2*D42</f>
+        <v>-0.00109147630966669</v>
       </c>
       <c r="D46" s="0" t="n">
-        <f aca="false">B33*B3*D42</f>
-        <v>0.000609750261333282</v>
+        <f aca="false">-B33*B3*D42</f>
+        <v>-0.00272869077416673</v>
       </c>
       <c r="F46" s="0" t="n">
         <f aca="false">C7+C46</f>
-        <v>1.00024390010453</v>
+        <v>0.998908523690333</v>
       </c>
       <c r="G46" s="0" t="n">
         <f aca="false">D7+D46</f>
-        <v>2.00060975026133</v>
+        <v>1.99727130922583</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C49" s="0" t="n">
-        <f aca="false">D39*C10*B33</f>
-        <v>-0.000627777344726821</v>
+        <f aca="false">-D39*C10*B33</f>
+        <v>0.000348699909895248</v>
       </c>
       <c r="D49" s="0" t="n">
-        <f aca="false">D39*C10*B33</f>
-        <v>-0.000627777344726821</v>
+        <f aca="false">-D39*C10*B33</f>
+        <v>0.000348699909895248</v>
       </c>
       <c r="F49" s="0" t="n">
         <f aca="false">C14+C49</f>
-        <v>-1.00062777734473</v>
+        <v>-0.999651300090105</v>
       </c>
       <c r="G49" s="0" t="n">
         <f aca="false">D14+D49</f>
-        <v>1.99937222265527</v>
+        <v>2.0003486999099</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C50" s="0" t="n">
-        <f aca="false">E39*C10*B33</f>
-        <v>-0.00103067013544835</v>
+        <f aca="false">-E39*C10*B33</f>
+        <v>0.00106708711404666</v>
       </c>
       <c r="D50" s="0" t="n">
-        <f aca="false">E39*C11*B33</f>
-        <v>-0.0013788943532605</v>
+        <f aca="false">-E39*C11*B33</f>
+        <v>0.00305370262283488</v>
       </c>
       <c r="F50" s="0" t="n">
         <f aca="false">C15+C50</f>
-        <v>0.998969329864552</v>
+        <v>1.00106708711405</v>
       </c>
       <c r="G50" s="0" t="n">
         <f aca="false">D15+D50</f>
-        <v>0.998621105646739</v>
+        <v>1.00305370262283</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C51" s="0" t="n">
-        <f aca="false">F39*C10*B33</f>
-        <v>-0.00311206924703967</v>
+        <f aca="false">-F39*C10*B33</f>
+        <v>0.003488308799942</v>
       </c>
       <c r="D51" s="0" t="n">
-        <f aca="false">F39*C11*B33</f>
-        <v>-0.00416351901943092</v>
+        <f aca="false">-F39*C11*B33</f>
+        <v>0.00998255680479999</v>
       </c>
       <c r="F51" s="0" t="n">
         <f aca="false">C16+C51</f>
-        <v>2.99688793075296</v>
+        <v>3.00348830879994</v>
       </c>
       <c r="G51" s="0" t="n">
         <f aca="false">D16+D51</f>
-        <v>-2.00416351901943</v>
+        <v>-1.9900174431952</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F53" s="2"/>
-      <c r="H53" s="6" t="s">
-        <v>30</v>
+      <c r="A53" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F53" s="3"/>
+      <c r="H53" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>18</v>
+      <c r="A54" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D54" s="0" t="n">
-        <f aca="false">B36*C19*B33</f>
-        <v>-0.00395447961726575</v>
+        <f aca="false">-B36*C19*B33</f>
+        <v>0.00467128763134758</v>
       </c>
       <c r="E54" s="0" t="n">
-        <f aca="false">B36*C20*B33</f>
-        <v>-0.00433336777240691</v>
+        <f aca="false">-B36*C20*B33</f>
+        <v>0.00429568570067348</v>
       </c>
       <c r="F54" s="0" t="n">
-        <f aca="false">B36*C21*B33</f>
-        <v>-0.00298609374228151</v>
+        <f aca="false">-B36*C21*B33</f>
+        <v>-0.00350493043444114</v>
       </c>
       <c r="H54" s="0" t="n">
         <f aca="false">D24+D54</f>
-        <v>0.996045520382734</v>
+        <v>1.00467128763135</v>
       </c>
       <c r="I54" s="0" t="n">
         <f aca="false">E24+E54</f>
-        <v>1.99566663222759</v>
+        <v>2.00429568570067</v>
       </c>
       <c r="J54" s="0" t="n">
         <f aca="false">F24+F54</f>
-        <v>3.99701390625772</v>
+        <v>3.99649506956556</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -879,534 +1163,587 @@
   </sheetPr>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L21" activeCellId="0" sqref="L21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.2</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
+      <c r="A5" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">Step_1!F45</f>
-        <v>-1.00082890942217</v>
+        <v>-0.992973689983025</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">Step_1!G45</f>
-        <v>0.997927726444576</v>
+        <v>1.01756577504244</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">Step_1!F46</f>
-        <v>1.00024390010453</v>
+        <v>0.998908523690333</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">Step_1!G46</f>
-        <v>2.00060975026133</v>
+        <v>1.99727130922583</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">C6*B2+D6*B3</f>
-        <v>0.298798081337854</v>
+        <v>0.310188149524613</v>
       </c>
       <c r="C10" s="0" t="n">
-        <f aca="false">1/(1+EXP(-B10))</f>
-        <v>0.574148671548628</v>
+        <f aca="false">TANH(B10)</f>
+        <v>0.300608254158304</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">1-C10*C10</f>
+        <v>0.909634677531896</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">C7*B2+D7*B3</f>
-        <v>1.20035365515157</v>
+        <v>1.19841735935098</v>
       </c>
       <c r="C11" s="0" t="n">
-        <f aca="false">1/(1+EXP(-B11))</f>
-        <v>0.768587690809729</v>
+        <f aca="false">TANH(B11)</f>
+        <v>0.833171232618558</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">1-C11*C11</f>
+        <v>0.305825697136872</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>12</v>
+      <c r="A13" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">Step_1!F49</f>
-        <v>-1.00062777734473</v>
+        <v>-0.999651300090105</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">Step_1!G49</f>
-        <v>1.99937222265527</v>
+        <v>2.0003486999099</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">Step_1!F50</f>
-        <v>0.998969329864552</v>
+        <v>1.00106708711405</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">Step_1!G50</f>
-        <v>0.998621105646739</v>
+        <v>1.00305370262283</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">Step_1!F51</f>
-        <v>2.99688793075296</v>
+        <v>3.00348830879994</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">Step_1!G51</f>
-        <v>-2.00416351901943</v>
+        <v>-1.9900174431952</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="4" t="s">
-        <v>9</v>
+      <c r="A18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">C14*C10+D14*C11</f>
-        <v>0.962183770602601</v>
+        <v>1.36612955988369</v>
       </c>
       <c r="C19" s="0" t="n">
-        <f aca="false">1/(1+EXP(-B19))</f>
-        <v>0.723558819273385</v>
+        <f aca="false">TANH(B19)</f>
+        <v>0.877807114284275</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">1-C19*C19</f>
+        <v>0.229454670111913</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B20" s="0" t="n">
         <f aca="false">C15*C10+D15*C11</f>
-        <v>1.34108480324244</v>
+        <v>1.13664451914957</v>
       </c>
       <c r="C20" s="0" t="n">
-        <f aca="false">1/(1+EXP(-B20))</f>
-        <v>0.792668280333359</v>
+        <f aca="false">TANH(B20)</f>
+        <v>0.813281111854509</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">1-C20*C20</f>
+        <v>0.338573833100693</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B21" s="0" t="n">
         <f aca="false">C16*C10+D16*C11</f>
-        <v>0.180283813133684</v>
+        <v>-0.755151909186148</v>
       </c>
       <c r="C21" s="0" t="n">
-        <f aca="false">1/(1+EXP(-B21))</f>
-        <v>0.544949273127789</v>
+        <f aca="false">TANH(B21)</f>
+        <v>-0.638212456699465</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">1-C21*C21</f>
+        <v>0.592684860113634</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>17</v>
+      <c r="A23" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D24" s="0" t="n">
         <f aca="false">Step_1!H54</f>
-        <v>0.996045520382734</v>
+        <v>1.00467128763135</v>
       </c>
       <c r="E24" s="0" t="n">
         <f aca="false">Step_1!I54</f>
-        <v>1.99566663222759</v>
+        <v>2.00429568570067</v>
       </c>
       <c r="F24" s="0" t="n">
         <f aca="false">Step_1!J54</f>
-        <v>3.99701390625772</v>
+        <v>3.99649506956556</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>9</v>
+      <c r="A26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B27" s="0" t="n">
         <f aca="false">D24*C19+E24*C20+F24*C21</f>
-        <v>4.480768981054</v>
+        <v>-0.0386495089829539</v>
       </c>
       <c r="C27" s="0" t="n">
-        <f aca="false">1/(1+EXP(-B27))</f>
-        <v>0.988802111418928</v>
+        <f aca="false">TANH(B27)</f>
+        <v>-0.0386302757952423</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">1-C27*C27</f>
+        <v>0.998507701791984</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B31" s="0" t="n">
-        <f aca="false">B29-C27</f>
-        <v>-0.588802111418928</v>
+        <f aca="false">C27-B29</f>
+        <v>-0.438630275795242</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="2" t="n">
-        <v>0.85</v>
+        <v>27</v>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>0.01</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
-        <v>23</v>
+      <c r="A35" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B36" s="0" t="n">
-        <f aca="false">B31*C27*(1-C27)</f>
-        <v>-0.00651950894834504</v>
+        <f aca="false">B31*D27</f>
+        <v>-0.437975708620691</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>25</v>
+      <c r="A38" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D39" s="0" t="n">
-        <f aca="false">B36*D24*C19*(1-C19)</f>
-        <v>-0.0012988848551636</v>
+        <f aca="false">B36*D24*D19</f>
+        <v>-0.10096501545986</v>
       </c>
       <c r="E39" s="0" t="n">
-        <f aca="false">B36*E24*C20*(1-C20)</f>
-        <v>-0.00213825802789032</v>
+        <f aca="false">B36*E24*D20</f>
+        <v>-0.297211223782634</v>
       </c>
       <c r="F39" s="0" t="n">
-        <f aca="false">B36*F24*C21*(1-C21)</f>
-        <v>-0.00646199228328522</v>
+        <f aca="false">B36*F24*D21</f>
+        <v>-1.03741647103759</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>28</v>
+      <c r="A41" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C42" s="0" t="n">
-        <f aca="false">(D39*C14+E39*C15+F39*C16)*C10*(1-C10)</f>
-        <v>-0.00493948282759145</v>
+        <f aca="false">(D39*C14+E39*C15+F39*C16)*D10</f>
+        <v>-3.01313467600203</v>
       </c>
       <c r="D42" s="0" t="n">
-        <f aca="false">(D39*D14+E39*D15+F39*D16)*C11*(1-C11)</f>
-        <v>0.00146177005698042</v>
+        <f aca="false">(D39*D14+E39*D15+F39*D16)*D11</f>
+        <v>0.478431523957409</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>30</v>
+      <c r="A44" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C45" s="0" t="n">
-        <f aca="false">B33*B2*C42</f>
-        <v>-0.000839712080690546</v>
+        <f aca="false">-B33*B2*C42</f>
+        <v>0.00602626935200405</v>
       </c>
       <c r="D45" s="0" t="n">
-        <f aca="false">B33*B3*C42</f>
-        <v>-0.00209928020172637</v>
+        <f aca="false">-B33*B3*C42</f>
+        <v>0.0150656733800101</v>
       </c>
       <c r="F45" s="0" t="n">
         <f aca="false">C6+C45</f>
-        <v>-1.00166862150286</v>
+        <v>-0.986947420631021</v>
       </c>
       <c r="G45" s="0" t="n">
         <f aca="false">D6+D45</f>
-        <v>0.995828446242849</v>
+        <v>1.03263144842245</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C46" s="0" t="n">
-        <f aca="false">B33*B2*D42</f>
-        <v>0.000248500909686671</v>
+        <f aca="false">-B33*B2*D42</f>
+        <v>-0.000956863047914817</v>
       </c>
       <c r="D46" s="0" t="n">
-        <f aca="false">B33*B3*D42</f>
-        <v>0.000621252274216678</v>
+        <f aca="false">-B33*B3*D42</f>
+        <v>-0.00239215761978704</v>
       </c>
       <c r="F46" s="0" t="n">
         <f aca="false">C7+C46</f>
-        <v>1.00049240101422</v>
+        <v>0.997951660642418</v>
       </c>
       <c r="G46" s="0" t="n">
         <f aca="false">D7+D46</f>
-        <v>2.00123100253555</v>
+        <v>1.99487915160605</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C49" s="0" t="n">
-        <f aca="false">D39*C10*B33</f>
-        <v>-0.000633890061973793</v>
+        <f aca="false">-D39*C10*B33</f>
+        <v>0.000303509170284547</v>
       </c>
       <c r="D49" s="0" t="n">
-        <f aca="false">D39*C10*B33</f>
-        <v>-0.000633890061973793</v>
+        <f aca="false">-D39*C10*B33</f>
+        <v>0.000303509170284547</v>
       </c>
       <c r="F49" s="0" t="n">
         <f aca="false">C14+C49</f>
-        <v>-1.0012616674067</v>
+        <v>-0.99934779091982</v>
       </c>
       <c r="G49" s="0" t="n">
         <f aca="false">D14+D49</f>
-        <v>1.9987383325933</v>
+        <v>2.00065220908018</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C50" s="0" t="n">
-        <f aca="false">E39*C10*B33</f>
-        <v>-0.0010435263052202</v>
+        <f aca="false">-E39*C10*B33</f>
+        <v>0.000893441470975508</v>
       </c>
       <c r="D50" s="0" t="n">
-        <f aca="false">E39*C11*B33</f>
-        <v>-0.00139692298000985</v>
+        <f aca="false">-E39*C11*B33</f>
+        <v>0.00247627841667048</v>
       </c>
       <c r="F50" s="0" t="n">
         <f aca="false">C15+C50</f>
-        <v>0.997925803559332</v>
+        <v>1.00196052858502</v>
       </c>
       <c r="G50" s="0" t="n">
         <f aca="false">D15+D50</f>
-        <v>0.99722418266673</v>
+        <v>1.00552998103951</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C51" s="0" t="n">
-        <f aca="false">F39*C10*B33</f>
-        <v>-0.00315362264225484</v>
+        <f aca="false">-F39*C10*B33</f>
+        <v>0.00311855954193678</v>
       </c>
       <c r="D51" s="0" t="n">
-        <f aca="false">F39*C11*B33</f>
-        <v>-0.00422161656798441</v>
+        <f aca="false">-F39*C11*B33</f>
+        <v>0.00864345559913181</v>
       </c>
       <c r="F51" s="0" t="n">
         <f aca="false">C16+C51</f>
-        <v>2.99373430811071</v>
+        <v>3.00660686834188</v>
       </c>
       <c r="G51" s="0" t="n">
         <f aca="false">D16+D51</f>
-        <v>-2.00838513558742</v>
+        <v>-1.98137398759607</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F53" s="2"/>
-      <c r="H53" s="6" t="s">
-        <v>30</v>
+      <c r="A53" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F53" s="3"/>
+      <c r="H53" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>18</v>
+      <c r="A54" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D54" s="0" t="n">
-        <f aca="false">B36*C19*B33</f>
-        <v>-0.00400966096737078</v>
+        <f aca="false">-B36*C19*B33</f>
+        <v>0.0038445819291094</v>
       </c>
       <c r="E54" s="0" t="n">
-        <f aca="false">B36*C20*B33</f>
-        <v>-0.00439263675469722</v>
+        <f aca="false">-B36*C20*B33</f>
+        <v>0.00356197371272302</v>
       </c>
       <c r="F54" s="0" t="n">
-        <f aca="false">B36*C21*B33</f>
-        <v>-0.00301988141316813</v>
+        <f aca="false">-B36*C21*B33</f>
+        <v>-0.002795215529735</v>
       </c>
       <c r="H54" s="0" t="n">
         <f aca="false">D24+D54</f>
-        <v>0.992035859415364</v>
+        <v>1.00851586956046</v>
       </c>
       <c r="I54" s="0" t="n">
         <f aca="false">E24+E54</f>
-        <v>1.9912739954729</v>
+        <v>2.0078576594134</v>
       </c>
       <c r="J54" s="0" t="n">
         <f aca="false">F24+F54</f>
-        <v>3.99399402484455</v>
+        <v>3.99369985403582</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1415,4 +1752,600 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <f aca="false">Step_2!F45</f>
+        <v>-0.986947420631021</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">Step_2!G45</f>
+        <v>1.03263144842245</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <f aca="false">Step_2!F46</f>
+        <v>0.997951660642418</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">Step_2!G46</f>
+        <v>1.99487915160605</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">C6*B2+D6*B3</f>
+        <v>0.318926240085019</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <f aca="false">TANH(B10)</f>
+        <v>0.308535699229749</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">1-C10*C10</f>
+        <v>0.90480572230081</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">C7*B2+D7*B3</f>
+        <v>1.19702990793151</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <f aca="false">TANH(B11)</f>
+        <v>0.832746423520763</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">1-C11*C11</f>
+        <v>0.306533394113377</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <f aca="false">Step_2!F49</f>
+        <v>-0.99934779091982</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">Step_2!G49</f>
+        <v>2.00065220908018</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <f aca="false">Step_2!F50</f>
+        <v>1.00196052858502</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">Step_2!G50</f>
+        <v>1.00552998103951</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <f aca="false">Step_2!F51</f>
+        <v>3.00660686834188</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">Step_2!G51</f>
+        <v>-1.98137398759607</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <f aca="false">C14*C10+D14*C11</f>
+        <v>1.35770150237528</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <f aca="false">TANH(B19)</f>
+        <v>0.875858889886677</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">1-C19*C19</f>
+        <v>0.232871205006478</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <f aca="false">C15*C10+D15*C11</f>
+        <v>1.14649208774114</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <f aca="false">TANH(B20)</f>
+        <v>0.816588644479749</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">1-C20*C20</f>
+        <v>0.333182985706725</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <f aca="false">C16*C10+D16*C11</f>
+        <v>-0.72233654939487</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <f aca="false">TANH(B21)</f>
+        <v>-0.618354529271497</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">1-C21*C21</f>
+        <v>0.617637676129425</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">Step_2!H54</f>
+        <v>1.00851586956046</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <f aca="false">Step_2!I54</f>
+        <v>2.0078576594134</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <f aca="false">Step_2!J54</f>
+        <v>3.99369985403582</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <f aca="false">D24*C19+E24*C20+F24*C21</f>
+        <v>0.0533889610610161</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <f aca="false">TANH(B27)</f>
+        <v>0.0533382925337684</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">1-C27*C27</f>
+        <v>0.997155026549582</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <f aca="false">C27-B29</f>
+        <v>-0.346661707466232</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <f aca="false">B31*D27</f>
+        <v>-0.345675464112214</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <f aca="false">B36*D24*D19</f>
+        <v>-0.0811833711605567</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <f aca="false">B36*E24*D20</f>
+        <v>-0.231251358084218</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <f aca="false">B36*F24*D21</f>
+        <v>-0.852663666434041</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <f aca="false">(D39*C14+E39*C15+F39*C16)*D10</f>
+        <v>-2.45582255705918</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <f aca="false">(D39*D14+E39*D15+F39*D16)*D11</f>
+        <v>0.396806174158849</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <f aca="false">-B33*B2*C42</f>
+        <v>0.00491164511411836</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <f aca="false">-B33*B3*C42</f>
+        <v>0.0122791127852959</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <f aca="false">C6+C45</f>
+        <v>-0.982035775516903</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <f aca="false">D6+D45</f>
+        <v>1.04491056120774</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <f aca="false">-B33*B2*D42</f>
+        <v>-0.000793612348317699</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <f aca="false">-B33*B3*D42</f>
+        <v>-0.00198403087079425</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <f aca="false">C7+C46</f>
+        <v>0.997158048294101</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <f aca="false">D7+D46</f>
+        <v>1.99289512073525</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <f aca="false">-D39*C10*B33</f>
+        <v>0.000250479681868506</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <f aca="false">-D39*C10*B33</f>
+        <v>0.000250479681868506</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <f aca="false">C14+C49</f>
+        <v>-0.999097311237952</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <f aca="false">D14+D49</f>
+        <v>2.00090268876205</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <f aca="false">-E39*C10*B33</f>
+        <v>0.000713492994643434</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <f aca="false">-E39*C11*B33</f>
+        <v>0.00192573741378952</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <f aca="false">C15+C50</f>
+        <v>1.00267402157967</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <f aca="false">D15+D50</f>
+        <v>1.00745571845329</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <f aca="false">-F39*C10*B33</f>
+        <v>0.00263077180531029</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <f aca="false">-F39*C11*B33</f>
+        <v>0.00710052618689049</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <f aca="false">C16+C51</f>
+        <v>3.00923764014719</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <f aca="false">D16+D51</f>
+        <v>-1.97427346140918</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F53" s="3"/>
+      <c r="H53" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <f aca="false">-B36*C19*B33</f>
+        <v>0.00302762928258385</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <f aca="false">-B36*C20*B33</f>
+        <v>0.00282274658669301</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <f aca="false">-B36*C21*B33</f>
+        <v>-0.00213749988891814</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <f aca="false">D24+D54</f>
+        <v>1.01154349884304</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <f aca="false">E24+E54</f>
+        <v>2.01068040600009</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <f aca="false">F24+F54</f>
+        <v>3.99156235414691</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update readme && inertia(as code, need to update excel)
</commit_message>
<xml_diff>
--- a/step_by_step_mlp.xlsx
+++ b/step_by_step_mlp.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="44">
   <si>
     <t xml:space="preserve">Input</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t xml:space="preserve">Learning Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Momentum (inertia)</t>
   </si>
   <si>
     <t xml:space="preserve">Error</t>
@@ -303,11 +300,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,11 +328,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -343,11 +340,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -431,14 +428,14 @@
   <dimension ref="A1:M80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M80" activeCellId="0" sqref="M80"/>
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.38"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.1"/>
@@ -844,20 +841,16 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>0.6</v>
-      </c>
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8"/>
+      <c r="A41" s="3"/>
       <c r="B41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B42" s="0" t="n">
         <f aca="false">C33-B36</f>
@@ -865,423 +858,178 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
+      <c r="A43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B45" s="9" t="n">
+      <c r="B45" s="0" t="n">
         <f aca="false">B42*D33</f>
         <v>-0.530796992035244</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
+      <c r="A46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B47" s="11"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B48" s="9" t="n">
+      <c r="B48" s="0" t="n">
         <f aca="false">H29*B45</f>
         <v>-0.530796992035244</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="9" t="n">
+      <c r="B49" s="0" t="n">
         <f aca="false">H30*B45</f>
         <v>-1.06159398407049</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B50" s="9" t="n">
+      <c r="B50" s="0" t="n">
         <f aca="false">H31*B45</f>
         <v>-2.12318796814098</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="9"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="F52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B53" s="9" t="n">
+      <c r="A53" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="0" t="n">
         <f aca="false">B48*D23</f>
         <v>-0.119699558134715</v>
       </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-      <c r="K53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="9" t="n">
+      <c r="A54" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="0" t="n">
         <f aca="false">B49*D24</f>
         <v>-0.366303094488909</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55" s="9" t="n">
+      <c r="A55" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="0" t="n">
         <f aca="false">B50*D25</f>
         <v>-1.19744516743904</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
-      <c r="K56" s="9"/>
+      <c r="A56" s="3"/>
+      <c r="F56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B57" s="11"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B58" s="9" t="n">
+      <c r="B58" s="0" t="n">
         <f aca="false">F17*B53+G17*B54+H17*B55</f>
         <v>-3.83893903867132</v>
       </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9"/>
-      <c r="K58" s="9"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="9" t="n">
+      <c r="B59" s="0" t="n">
         <f aca="false">F18*B53+G18*B54+H18*B55</f>
         <v>1.78918812411974</v>
       </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="9"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="9"/>
-      <c r="K60" s="9"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="9"/>
-      <c r="J61" s="9"/>
-      <c r="K61" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="F61" s="3"/>
+      <c r="H61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B62" s="8" t="n">
+      <c r="A62" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" s="3" t="n">
         <f aca="false">B58*D12</f>
         <v>-3.51315500848731</v>
       </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9"/>
-      <c r="K62" s="9"/>
+      <c r="C62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B63" s="8" t="n">
+      <c r="A63" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="3" t="n">
         <f aca="false">B59*D13</f>
         <v>0.545738154833346</v>
       </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
-      <c r="J63" s="9"/>
-      <c r="K63" s="9"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="9"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
-      <c r="J64" s="9"/>
-      <c r="K64" s="9"/>
+      <c r="C63" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
-      <c r="J65" s="9"/>
-      <c r="K65" s="9"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B66" s="9" t="n">
+      <c r="B66" s="0" t="n">
         <f aca="false">F7*B62+G7*B63</f>
         <v>4.05889316332066</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
-      <c r="J66" s="9"/>
-      <c r="K66" s="9"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="9" t="s">
+      <c r="A67" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B67" s="9" t="n">
+      <c r="B67" s="0" t="n">
         <f aca="false">F8*B62+G8*B63</f>
         <v>-2.42167869882062</v>
       </c>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
-      <c r="J67" s="9"/>
-      <c r="K67" s="9"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="13"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
-      <c r="J68" s="9"/>
-      <c r="K68" s="9"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1290,26 +1038,16 @@
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
-      <c r="I69" s="9"/>
-      <c r="J69" s="9"/>
-      <c r="K69" s="9"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B70" s="14"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
       <c r="F70" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G70" s="15"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="9"/>
-      <c r="J70" s="9"/>
-      <c r="K70" s="9"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
@@ -1318,31 +1056,28 @@
       <c r="B71" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C71" s="9" t="n">
+      <c r="C71" s="0" t="n">
         <f aca="false">-($B$39*B2*B62)</f>
         <v>0.00702631001697462</v>
       </c>
-      <c r="D71" s="9" t="n">
+      <c r="D71" s="0" t="n">
         <f aca="false">-($B$39*B3*B62)</f>
         <v>0.0175657750424366</v>
       </c>
-      <c r="E71" s="9"/>
       <c r="F71" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G71" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="H71" s="9" t="n">
+      <c r="H71" s="0" t="n">
         <f aca="false">C71+C7</f>
         <v>-0.992973689983025</v>
       </c>
-      <c r="I71" s="9" t="n">
+      <c r="I71" s="0" t="n">
         <f aca="false">D71+D7</f>
         <v>1.01756577504244</v>
       </c>
-      <c r="J71" s="9"/>
-      <c r="K71" s="9"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
@@ -1351,59 +1086,38 @@
       <c r="B72" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C72" s="9" t="n">
+      <c r="C72" s="0" t="n">
         <f aca="false">-($B$39*B2*B63)</f>
         <v>-0.00109147630966669</v>
       </c>
-      <c r="D72" s="9" t="n">
+      <c r="D72" s="0" t="n">
         <f aca="false">-($B$39*B3*B63)</f>
         <v>-0.00272869077416673</v>
       </c>
-      <c r="E72" s="9"/>
       <c r="F72" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H72" s="9" t="n">
+      <c r="H72" s="0" t="n">
         <f aca="false">C72+C8</f>
         <v>0.998908523690333</v>
       </c>
-      <c r="I72" s="9" t="n">
+      <c r="I72" s="0" t="n">
         <f aca="false">D72+D8</f>
         <v>1.99727130922583</v>
       </c>
-      <c r="J72" s="9"/>
-      <c r="K72" s="9"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="9"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="9"/>
-      <c r="J73" s="9"/>
-      <c r="K73" s="9"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B74" s="14"/>
-      <c r="E74" s="9"/>
       <c r="F74" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G74" s="15"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
-      <c r="J74" s="9"/>
-      <c r="K74" s="9"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
@@ -1420,23 +1134,20 @@
         <f aca="false">-($B$39*$C$13*B53)</f>
         <v>0.000997880880963243</v>
       </c>
-      <c r="E75" s="9"/>
       <c r="F75" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G75" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="H75" s="9" t="n">
+      <c r="H75" s="0" t="n">
         <f aca="false">C75+C17</f>
         <v>-0.999651300090105</v>
       </c>
-      <c r="I75" s="9" t="n">
+      <c r="I75" s="0" t="n">
         <f aca="false">D75+D17</f>
         <v>2.00099788088096</v>
       </c>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
@@ -1453,23 +1164,20 @@
         <f aca="false">-($B$39*$C$13*B54)</f>
         <v>0.00305370262283488</v>
       </c>
-      <c r="E76" s="9"/>
       <c r="F76" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G76" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H76" s="9" t="n">
+      <c r="H76" s="0" t="n">
         <f aca="false">C76+C18</f>
         <v>1.00106708711405</v>
       </c>
-      <c r="I76" s="9" t="n">
+      <c r="I76" s="0" t="n">
         <f aca="false">D76+D18</f>
         <v>1.00305370262283</v>
       </c>
-      <c r="J76" s="9"/>
-      <c r="K76" s="9"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
@@ -1486,45 +1194,29 @@
         <f aca="false">-($B$39*$C$13*B55)</f>
         <v>0.00998255680479999</v>
       </c>
-      <c r="E77" s="9"/>
       <c r="F77" s="0" t="s">
         <v>20</v>
       </c>
       <c r="G77" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H77" s="9" t="n">
+      <c r="H77" s="0" t="n">
         <f aca="false">C77+C19</f>
         <v>3.00348830879994</v>
       </c>
-      <c r="I77" s="9" t="n">
+      <c r="I77" s="0" t="n">
         <f aca="false">D77+D19</f>
         <v>-1.9900174431952</v>
       </c>
-      <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="9"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9"/>
-      <c r="J78" s="9"/>
-      <c r="K78" s="9"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
       <c r="H79" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I79" s="15"/>
       <c r="J79" s="15"/>
@@ -1610,13 +1302,15 @@
   </sheetPr>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H46" activeCellId="0" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.89"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
@@ -2033,20 +1727,16 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>0.6</v>
-      </c>
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8"/>
+      <c r="A41" s="3"/>
       <c r="B41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B42" s="0" t="n">
         <f aca="false">C33-B36</f>
@@ -2054,423 +1744,178 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
+      <c r="A43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B45" s="9" t="n">
+      <c r="B45" s="0" t="n">
         <f aca="false">B42*D33</f>
         <v>-0.437855661178151</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
+      <c r="A46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B47" s="11"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B48" s="9" t="n">
+      <c r="B48" s="0" t="n">
         <f aca="false">H29*B45</f>
         <v>-0.439901010912528</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="9" t="n">
+      <c r="B49" s="0" t="n">
         <f aca="false">H30*B45</f>
         <v>-0.877592212658983</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B50" s="9" t="n">
+      <c r="B50" s="0" t="n">
         <f aca="false">H31*B45</f>
         <v>-1.74988799107985</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="9"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="F52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B53" s="9" t="n">
+      <c r="A53" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="0" t="n">
         <f aca="false">B48*D23</f>
         <v>-0.10084153251995</v>
       </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-      <c r="K53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="9" t="n">
+      <c r="A54" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="0" t="n">
         <f aca="false">B49*D24</f>
         <v>-0.297129759339271</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55" s="9" t="n">
+      <c r="A55" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="0" t="n">
         <f aca="false">B50*D25</f>
         <v>-1.03713211920769</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
-      <c r="K56" s="9"/>
+      <c r="A56" s="3"/>
+      <c r="F56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B57" s="11"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B58" s="9" t="n">
+      <c r="B58" s="0" t="n">
         <f aca="false">F17*B53+G17*B54+H17*B55</f>
         <v>-3.31165464831121</v>
       </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9"/>
-      <c r="K58" s="9"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="9" t="n">
+      <c r="B59" s="0" t="n">
         <f aca="false">F18*B53+G18*B54+H18*B55</f>
         <v>1.5640902099794</v>
       </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="9"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="9"/>
-      <c r="K60" s="9"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="9"/>
-      <c r="J61" s="9"/>
-      <c r="K61" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="F61" s="3"/>
+      <c r="H61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B62" s="8" t="n">
+      <c r="A62" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" s="3" t="n">
         <f aca="false">B58*D12</f>
         <v>-3.01239590811357</v>
       </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9"/>
-      <c r="K62" s="9"/>
+      <c r="C62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B63" s="8" t="n">
+      <c r="A63" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="3" t="n">
         <f aca="false">B59*D13</f>
         <v>0.478338978851908</v>
       </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
-      <c r="J63" s="9"/>
-      <c r="K63" s="9"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="9"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
-      <c r="J64" s="9"/>
-      <c r="K64" s="9"/>
+      <c r="C63" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
-      <c r="J65" s="9"/>
-      <c r="K65" s="9"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B66" s="9" t="n">
+      <c r="B66" s="0" t="n">
         <f aca="false">F7*B62+G7*B63</f>
         <v>3.4690467637578</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
-      <c r="J66" s="9"/>
-      <c r="K66" s="9"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="9" t="s">
+      <c r="A67" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B67" s="9" t="n">
+      <c r="B67" s="0" t="n">
         <f aca="false">F8*B62+G8*B63</f>
         <v>-2.10993825842895</v>
       </c>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
-      <c r="J67" s="9"/>
-      <c r="K67" s="9"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="13"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
-      <c r="J68" s="9"/>
-      <c r="K68" s="9"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -2479,26 +1924,16 @@
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
-      <c r="I69" s="9"/>
-      <c r="J69" s="9"/>
-      <c r="K69" s="9"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B70" s="14"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
       <c r="F70" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G70" s="15"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="9"/>
-      <c r="J70" s="9"/>
-      <c r="K70" s="9"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
@@ -2507,31 +1942,28 @@
       <c r="B71" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C71" s="9" t="n">
+      <c r="C71" s="0" t="n">
         <f aca="false">-($B$39*B2*B62)</f>
         <v>0.00602479181622714</v>
       </c>
-      <c r="D71" s="9" t="n">
+      <c r="D71" s="0" t="n">
         <f aca="false">-($B$39*B3*B62)</f>
         <v>0.0150619795405679</v>
       </c>
-      <c r="E71" s="9"/>
       <c r="F71" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G71" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="H71" s="9" t="n">
+      <c r="H71" s="0" t="n">
         <f aca="false">C71+C7</f>
         <v>-0.986948898166798</v>
       </c>
-      <c r="I71" s="9" t="n">
+      <c r="I71" s="0" t="n">
         <f aca="false">D71+D7</f>
         <v>1.032627754583</v>
       </c>
-      <c r="J71" s="9"/>
-      <c r="K71" s="9"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
@@ -2540,59 +1972,38 @@
       <c r="B72" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C72" s="9" t="n">
+      <c r="C72" s="0" t="n">
         <f aca="false">-($B$39*B2*B63)</f>
         <v>-0.000956677957703815</v>
       </c>
-      <c r="D72" s="9" t="n">
+      <c r="D72" s="0" t="n">
         <f aca="false">-($B$39*B3*B63)</f>
         <v>-0.00239169489425954</v>
       </c>
-      <c r="E72" s="9"/>
       <c r="F72" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H72" s="9" t="n">
+      <c r="H72" s="0" t="n">
         <f aca="false">C72+C8</f>
         <v>0.99795184573263</v>
       </c>
-      <c r="I72" s="9" t="n">
+      <c r="I72" s="0" t="n">
         <f aca="false">D72+D8</f>
         <v>1.99487961433157</v>
       </c>
-      <c r="J72" s="9"/>
-      <c r="K72" s="9"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="9"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="9"/>
-      <c r="J73" s="9"/>
-      <c r="K73" s="9"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B74" s="14"/>
-      <c r="E74" s="9"/>
       <c r="F74" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G74" s="15"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
-      <c r="J74" s="9"/>
-      <c r="K74" s="9"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
@@ -2609,23 +2020,20 @@
         <f aca="false">-($B$39*$C$13*B53)</f>
         <v>0.000840182639487912</v>
       </c>
-      <c r="E75" s="9"/>
       <c r="F75" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G75" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="H75" s="9" t="n">
+      <c r="H75" s="0" t="n">
         <f aca="false">C75+C17</f>
         <v>-0.99934816211973</v>
       </c>
-      <c r="I75" s="9" t="n">
+      <c r="I75" s="0" t="n">
         <f aca="false">D75+D17</f>
         <v>2.00183806352045</v>
       </c>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
@@ -2642,23 +2050,20 @@
         <f aca="false">-($B$39*$C$13*B54)</f>
         <v>0.00247559967836356</v>
       </c>
-      <c r="E76" s="9"/>
       <c r="F76" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G76" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H76" s="9" t="n">
+      <c r="H76" s="0" t="n">
         <f aca="false">C76+C18</f>
         <v>1.00196028369618</v>
       </c>
-      <c r="I76" s="9" t="n">
+      <c r="I76" s="0" t="n">
         <f aca="false">D76+D18</f>
         <v>1.0055293023012</v>
       </c>
-      <c r="J76" s="9"/>
-      <c r="K76" s="9"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
@@ -2675,45 +2080,29 @@
         <f aca="false">-($B$39*$C$13*B55)</f>
         <v>0.00864108646148566</v>
       </c>
-      <c r="E77" s="9"/>
       <c r="F77" s="0" t="s">
         <v>20</v>
       </c>
       <c r="G77" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H77" s="9" t="n">
+      <c r="H77" s="0" t="n">
         <f aca="false">C77+C19</f>
         <v>3.00660601355681</v>
       </c>
-      <c r="I77" s="9" t="n">
+      <c r="I77" s="0" t="n">
         <f aca="false">D77+D19</f>
         <v>-1.98137635673371</v>
       </c>
-      <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="9"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9"/>
-      <c r="J78" s="9"/>
-      <c r="K78" s="9"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
       <c r="H79" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I79" s="15"/>
       <c r="J79" s="15"/>
@@ -2799,13 +2188,15 @@
   </sheetPr>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M66" activeCellId="0" sqref="M66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K46" activeCellId="0" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3220,20 +2611,15 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>0.6</v>
-      </c>
+      <c r="A40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8"/>
+      <c r="A41" s="3"/>
       <c r="B41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B42" s="0" t="n">
         <f aca="false">C33-B36</f>
@@ -3241,423 +2627,178 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
+      <c r="A43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B45" s="9" t="n">
+      <c r="B45" s="0" t="n">
         <f aca="false">B42*D33</f>
         <v>-0.34546045071471</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
+      <c r="A46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B47" s="11"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B48" s="9" t="n">
+      <c r="B48" s="0" t="n">
         <f aca="false">H29*B45</f>
         <v>-0.348402170447938</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="9" t="n">
+      <c r="B49" s="0" t="n">
         <f aca="false">H30*B45</f>
         <v>-0.69363507471089</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B50" s="9" t="n">
+      <c r="B50" s="0" t="n">
         <f aca="false">H31*B45</f>
         <v>-1.37966561627168</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="9"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="F52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B53" s="9" t="n">
+      <c r="A53" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="0" t="n">
         <f aca="false">B48*D23</f>
         <v>-0.0809923065782294</v>
       </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-      <c r="K53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="9" t="n">
+      <c r="A54" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="0" t="n">
         <f aca="false">B49*D24</f>
         <v>-0.231108348908498</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55" s="9" t="n">
+      <c r="A55" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="0" t="n">
         <f aca="false">B50*D25</f>
         <v>-0.852124794204125</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
-      <c r="K56" s="9"/>
+      <c r="A56" s="3"/>
+      <c r="F56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B57" s="11"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B58" s="9" t="n">
+      <c r="B58" s="0" t="n">
         <f aca="false">F17*B53+G17*B54+H17*B55</f>
         <v>-2.7126254046671</v>
       </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9"/>
-      <c r="K58" s="9"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="9" t="n">
+      <c r="B59" s="0" t="n">
         <f aca="false">F18*B53+G18*B54+H18*B55</f>
         <v>1.29386022122807</v>
       </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="9"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="9"/>
-      <c r="K60" s="9"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="9"/>
-      <c r="J61" s="9"/>
-      <c r="K61" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="F61" s="3"/>
+      <c r="H61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B62" s="8" t="n">
+      <c r="A62" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" s="3" t="n">
         <f aca="false">B58*D12</f>
         <v>-2.45440223338325</v>
       </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9"/>
-      <c r="K62" s="9"/>
+      <c r="C62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B63" s="8" t="n">
+      <c r="A63" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="3" t="n">
         <f aca="false">B59*D13</f>
         <v>0.396611187841506</v>
       </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
-      <c r="J63" s="9"/>
-      <c r="K63" s="9"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="9"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
-      <c r="J64" s="9"/>
-      <c r="K64" s="9"/>
+      <c r="C63" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
-      <c r="J65" s="9"/>
-      <c r="K65" s="9"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B66" s="9" t="n">
+      <c r="B66" s="0" t="n">
         <f aca="false">F7*B62+G7*B63</f>
         <v>2.81816844684037</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
-      <c r="J66" s="9"/>
-      <c r="K66" s="9"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="9" t="s">
+      <c r="A67" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B67" s="9" t="n">
+      <c r="B67" s="0" t="n">
         <f aca="false">F8*B62+G8*B63</f>
         <v>-1.7432922936612</v>
       </c>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
-      <c r="J67" s="9"/>
-      <c r="K67" s="9"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="13"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
-      <c r="J68" s="9"/>
-      <c r="K68" s="9"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -3666,26 +2807,16 @@
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
-      <c r="I69" s="9"/>
-      <c r="J69" s="9"/>
-      <c r="K69" s="9"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B70" s="14"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
       <c r="F70" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G70" s="15"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="9"/>
-      <c r="J70" s="9"/>
-      <c r="K70" s="9"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
@@ -3694,31 +2825,28 @@
       <c r="B71" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C71" s="9" t="n">
+      <c r="C71" s="0" t="n">
         <f aca="false">-($B$39*B2*B62)</f>
         <v>0.00490880446676649</v>
       </c>
-      <c r="D71" s="9" t="n">
+      <c r="D71" s="0" t="n">
         <f aca="false">-($B$39*B3*B62)</f>
         <v>0.0122720111669162</v>
       </c>
-      <c r="E71" s="9"/>
       <c r="F71" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G71" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="H71" s="9" t="n">
+      <c r="H71" s="0" t="n">
         <f aca="false">C71+C7</f>
         <v>-0.982040093700032</v>
       </c>
-      <c r="I71" s="9" t="n">
+      <c r="I71" s="0" t="n">
         <f aca="false">D71+D7</f>
         <v>1.04489976574992</v>
       </c>
-      <c r="J71" s="9"/>
-      <c r="K71" s="9"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
@@ -3727,59 +2855,38 @@
       <c r="B72" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C72" s="9" t="n">
+      <c r="C72" s="0" t="n">
         <f aca="false">-($B$39*B2*B63)</f>
         <v>-0.000793222375683012</v>
       </c>
-      <c r="D72" s="9" t="n">
+      <c r="D72" s="0" t="n">
         <f aca="false">-($B$39*B3*B63)</f>
         <v>-0.00198305593920753</v>
       </c>
-      <c r="E72" s="9"/>
       <c r="F72" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H72" s="9" t="n">
+      <c r="H72" s="0" t="n">
         <f aca="false">C72+C8</f>
         <v>0.997158623356946</v>
       </c>
-      <c r="I72" s="9" t="n">
+      <c r="I72" s="0" t="n">
         <f aca="false">D72+D8</f>
         <v>1.99289655839237</v>
       </c>
-      <c r="J72" s="9"/>
-      <c r="K72" s="9"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="9"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="9"/>
-      <c r="J73" s="9"/>
-      <c r="K73" s="9"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B74" s="14"/>
-      <c r="E74" s="9"/>
       <c r="F74" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G74" s="15"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
-      <c r="J74" s="9"/>
-      <c r="K74" s="9"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
@@ -3796,23 +2903,20 @@
         <f aca="false">-($B$39*$C$13*B53)</f>
         <v>0.000674460602987654</v>
       </c>
-      <c r="E75" s="9"/>
       <c r="F75" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G75" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="H75" s="9" t="n">
+      <c r="H75" s="0" t="n">
         <f aca="false">C75+C17</f>
         <v>-0.999098273510327</v>
       </c>
-      <c r="I75" s="9" t="n">
+      <c r="I75" s="0" t="n">
         <f aca="false">D75+D17</f>
         <v>2.00251252412344</v>
       </c>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
@@ -3829,23 +2933,20 @@
         <f aca="false">-($B$39*$C$13*B54)</f>
         <v>0.00192454670012084</v>
       </c>
-      <c r="E76" s="9"/>
       <c r="F76" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G76" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H76" s="9" t="n">
+      <c r="H76" s="0" t="n">
         <f aca="false">C76+C18</f>
         <v>1.00267333097647</v>
       </c>
-      <c r="I76" s="9" t="n">
+      <c r="I76" s="0" t="n">
         <f aca="false">D76+D18</f>
         <v>1.00745384900132</v>
       </c>
-      <c r="J76" s="9"/>
-      <c r="K76" s="9"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
@@ -3862,45 +2963,29 @@
         <f aca="false">-($B$39*$C$13*B55)</f>
         <v>0.00709603944869165</v>
       </c>
-      <c r="E77" s="9"/>
       <c r="F77" s="0" t="s">
         <v>20</v>
       </c>
       <c r="G77" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H77" s="9" t="n">
+      <c r="H77" s="0" t="n">
         <f aca="false">C77+C19</f>
         <v>3.00923510623063</v>
       </c>
-      <c r="I77" s="9" t="n">
+      <c r="I77" s="0" t="n">
         <f aca="false">D77+D19</f>
         <v>-1.97428031728502</v>
       </c>
-      <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="9"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9"/>
-      <c r="J78" s="9"/>
-      <c r="K78" s="9"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
       <c r="H79" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I79" s="15"/>
       <c r="J79" s="15"/>

</xml_diff>